<commit_message>
reverting few columns from isoptional to isrequired and also including metaEDD output
</commit_message>
<xml_diff>
--- a/ArizonaExtensions/MetaEdOutput/Documentation/Ed-Fi-Handbook/Ed-Fi-Handbook.xlsx
+++ b/ArizonaExtensions/MetaEdOutput/Documentation/Ed-Fi-Handbook/Ed-Fi-Handbook.xlsx
@@ -2613,6 +2613,7 @@
 Student (identity)
 Used By:
 StudentSchoolAssociationLocalEducationAgency.StudentSchoolAssociation (as identity)
+StudentSchoolAssociationMembershipFTE.StudentSchoolAssociation (as identity)
 StudentSchoolAssociationSpecialEnrollment.StudentSchoolAssociation (as identity)
 StudentSchoolAssociationTuitionPayer.StudentSchoolAssociation (as identity)</v>
       </c>
@@ -38124,7 +38125,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I648" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.StudentDropOutRecoveryProgramAssociation
+        <v xml:space="preserve">arizona.StudentDropOutRecoveryProgramAssociation
 BeginDate [DATE] NOT NULL
 EducationOrganizationId [INT] NOT NULL
 ProgramEducationOrganizationId [INT] NOT NULL
@@ -38164,7 +38165,7 @@
       </c>
       <c r="G649" t="str" xml:space="preserve">
         <v xml:space="preserve">Used By:
-StudentSectionAssociation.DualCredit (as optional)</v>
+StudentSectionAssociation.DualCredit (as required)</v>
       </c>
       <c r="H649" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="DualCredit"&gt;
@@ -38201,7 +38202,7 @@
       </c>
       <c r="G650" t="str" xml:space="preserve">
         <v xml:space="preserve">Used By:
-StudentSectionAssociation.ConcurrentEnrollment (as optional)</v>
+StudentSectionAssociation.ConcurrentEnrollment (as required)</v>
       </c>
       <c r="H650" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="ConcurrentEnrollment"&gt;
@@ -39258,7 +39259,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I676" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.AbsenceAmountDescriptor
+        <v xml:space="preserve">arizona.AbsenceAmountDescriptor
 AbsenceAmountDescriptorId [INT] NOT NULL
 Primary Keys:
 AbsenceAmountDescriptorId
@@ -39306,7 +39307,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I677" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.CourseEntryDescriptor
+        <v xml:space="preserve">arizona.CourseEntryDescriptor
 CourseEntryDescriptorId [INT] NOT NULL
 Primary Keys:
 CourseEntryDescriptorId
@@ -39350,7 +39351,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I678" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.CourseExitDescriptor
+        <v xml:space="preserve">arizona.CourseExitDescriptor
 CourseExitDescriptorId [INT] NOT NULL
 Primary Keys:
 CourseExitDescriptorId
@@ -39362,7 +39363,7 @@
         <v/>
       </c>
       <c r="B679" t="str">
-        <v>EndOfCourseAssessmentCodeType</v>
+        <v>EndOfCourseAssessmentCode</v>
       </c>
       <c r="C679" t="str">
         <v>Submitted for courses that end with Assessment testing</v>
@@ -39378,10 +39379,10 @@
       </c>
       <c r="G679" t="str" xml:space="preserve">
         <v xml:space="preserve">Used By:
-CourseOffering.EndOfCourseAssessmentCodeType (as optional)</v>
+CourseOffering.EndOfCourseAssessmentCode (as optional)</v>
       </c>
       <c r="H679" t="str" xml:space="preserve">
-        <v xml:space="preserve">&lt;xs:complexType name="EXTENSION-EndOfCourseAssessmentCodeTypeDescriptor"&gt;
+        <v xml:space="preserve">&lt;xs:complexType name="EXTENSION-EndOfCourseAssessmentCodeDescriptor"&gt;
   &lt;xs:annotation&gt;
     &lt;xs:documentation&gt;Submitted for courses that end with Assessment testing&lt;/xs:documentation&gt;
     &lt;xs:appinfo&gt;
@@ -39394,10 +39395,10 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I679" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.EndOfCourseAssessmentCodeTypeDescriptor
-EndOfCourseAssessmentCodeTypeDescriptorId [INT] NOT NULL
-Primary Keys:
-EndOfCourseAssessmentCodeTypeDescriptorId
+        <v xml:space="preserve">arizona.EndOfCourseAssessmentCodeDescriptor
+EndOfCourseAssessmentCodeDescriptorId [INT] NOT NULL
+Primary Keys:
+EndOfCourseAssessmentCodeDescriptorId
 </v>
       </c>
     </row>
@@ -39446,7 +39447,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I680" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.ExitWithdrawReasonDescriptor
+        <v xml:space="preserve">arizona.ExitWithdrawReasonDescriptor
 ExitWithdrawReasonDescriptorId [INT] NOT NULL
 Primary Keys:
 ExitWithdrawReasonDescriptorId
@@ -39490,7 +39491,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I681" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.MembershipFTEDescriptor
+        <v xml:space="preserve">arizona.MembershipFTEDescriptor
 MembershipFTEDescriptorId [INT] NOT NULL
 Primary Keys:
 MembershipFTEDescriptorId
@@ -39534,7 +39535,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I682" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.MembershipResponsibilityDescriptor
+        <v xml:space="preserve">arizona.MembershipResponsibilityDescriptor
 MembershipResponsibilityDescriptorId [INT] NOT NULL
 Primary Keys:
 MembershipResponsibilityDescriptorId
@@ -39584,7 +39585,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I683" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.MembershipTypeDescriptor
+        <v xml:space="preserve">arizona.MembershipTypeDescriptor
 MembershipTypeDescriptorId [INT] NOT NULL
 Primary Keys:
 MembershipTypeDescriptorId
@@ -39628,7 +39629,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I684" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.MonthDescriptor
+        <v xml:space="preserve">arizona.MonthDescriptor
 MonthDescriptorId [INT] NOT NULL
 Primary Keys:
 MonthDescriptorId
@@ -39672,7 +39673,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I685" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.NumberOfInstructionalDaysInWeekDescriptor
+        <v xml:space="preserve">arizona.NumberOfInstructionalDaysInWeekDescriptor
 NumberOfInstructionalDaysInWeekDescriptorId [INT] NOT NULL
 Primary Keys:
 NumberOfInstructionalDaysInWeekDescriptorId
@@ -39718,7 +39719,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I686" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.PrimaryNightTimeResidenceDescriptor
+        <v xml:space="preserve">arizona.PrimaryNightTimeResidenceDescriptor
 PrimaryNightTimeResidenceDescriptorId [INT] NOT NULL
 Primary Keys:
 PrimaryNightTimeResidenceDescriptorId
@@ -39766,7 +39767,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I687" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.SessionTypeDescriptor
+        <v xml:space="preserve">arizona.SessionTypeDescriptor
 SessionTypeDescriptorId [INT] NOT NULL
 Primary Keys:
 SessionTypeDescriptorId
@@ -39810,7 +39811,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I688" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.SpecialEnrollmentDescriptor
+        <v xml:space="preserve">arizona.SpecialEnrollmentDescriptor
 SpecialEnrollmentDescriptorId [INT] NOT NULL
 Primary Keys:
 SpecialEnrollmentDescriptorId
@@ -39867,7 +39868,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I689" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.StudentNeedDescriptor
+        <v xml:space="preserve">arizona.StudentNeedDescriptor
 StudentNeedDescriptorId [INT] NOT NULL
 StudentNeedCategoryDescriptorId [INT] NOT NULL
 Primary Keys:
@@ -39912,7 +39913,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I690" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.StudentNeedCategoryDescriptor
+        <v xml:space="preserve">arizona.StudentNeedCategoryDescriptor
 StudentNeedCategoryDescriptorId [INT] NOT NULL
 Primary Keys:
 StudentNeedCategoryDescriptorId
@@ -39960,7 +39961,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I691" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.TrackEventDescriptor
+        <v xml:space="preserve">arizona.TrackEventDescriptor
 TrackEventDescriptorId [INT] NOT NULL
 Primary Keys:
 TrackEventDescriptorId
@@ -40004,7 +40005,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I692" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.TrackNumberDescriptor
+        <v xml:space="preserve">arizona.TrackNumberDescriptor
 TrackNumberDescriptorId [INT] NOT NULL
 Primary Keys:
 TrackNumberDescriptorId
@@ -40048,7 +40049,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I693" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.TuitionPayerDescriptor
+        <v xml:space="preserve">arizona.TuitionPayerDescriptor
 TuitionPayerDescriptorId [INT] NOT NULL
 Primary Keys:
 TuitionPayerDescriptorId
@@ -40128,7 +40129,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I694" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.CalendarDateTrackEvent
+        <v xml:space="preserve">arizona.CalendarDateTrackEvent
 Date [DATE] NOT NULL
 TrackEventDescriptorId [INT] NOT NULL
 TrackLocalEducationAgencyId [INT] NOT NULL
@@ -40219,7 +40220,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I695" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.StudentDropOutRecoveryProgramMonthlyUpdate
+        <v xml:space="preserve">arizona.StudentDropOutRecoveryProgramMonthlyUpdate
 BeginDate [DATE] NOT NULL
 EducationOrganizationId [INT] NOT NULL
 MonthDescriptorId [INT] NOT NULL
@@ -40333,7 +40334,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I696" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.StudentNeed
+        <v xml:space="preserve">arizona.StudentNeed
 EducationOrganizationId [INT] NOT NULL
 StudentNeedDescriptorId [INT] NOT NULL
 StudentNeedEntryDate [DATE] NOT NULL
@@ -40424,7 +40425,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I697" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.StudentSchoolAssociationLocalEducationAgency
+        <v xml:space="preserve">arizona.StudentSchoolAssociationLocalEducationAgency
 EntryDate [DATE] NOT NULL
 MembershipResponsibilityDescriptorId [INT] NOT NULL
 SchoolId [INT] NOT NULL
@@ -40467,7 +40468,8 @@
         <v xml:space="preserve">Contains:
 FTEEndDate (optional)
 FTEStartDate (identity)
-MembershipFTE (required)</v>
+MembershipFTE (required)
+StudentSchoolAssociation (identity)</v>
       </c>
       <c r="H698" t="str" xml:space="preserve">
         <v xml:space="preserve">&lt;xs:complexType name="EXTENSION-StudentSchoolAssociationMembershipFTE"&gt;
@@ -40480,6 +40482,11 @@
   &lt;xs:complexContent&gt;
     &lt;xs:extension base="ComplexObjectType"&gt;
       &lt;xs:sequence&gt;
+        &lt;xs:element name="StudentSchoolAssociationReference" type="StudentSchoolAssociationReferenceType"&gt;
+          &lt;xs:annotation&gt;
+            &lt;xs:documentation&gt;The reference to StudentSchoolAssociation&lt;/xs:documentation&gt;
+          &lt;/xs:annotation&gt;
+        &lt;/xs:element&gt;
         &lt;xs:element name="FTEStartDate" type="xs:date"&gt;
           &lt;xs:annotation&gt;
             &lt;xs:documentation&gt;The start date for the StudentSchoolAssociationMembership&lt;/xs:documentation&gt;
@@ -40504,15 +40511,21 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I698" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.StudentSchoolAssociationMembershipFTE
+        <v xml:space="preserve">arizona.StudentSchoolAssociationMembershipFTE
+EntryDate [DATE] NOT NULL
 FTEStartDate [DATE] NOT NULL
+SchoolId [INT] NOT NULL
+StudentUSI [INT] NOT NULL
 FTEEndDate [DATE] NULL
 MembershipFTEDescriptorId [INT] NOT NULL
 CreateDate [DATETIME] NOT NULL
 LastModifiedDate [DATETIME] NOT NULL
 Id [UNIQUEIDENTIFIER] NOT NULL
 Primary Keys:
+EntryDate
 FTEStartDate
+SchoolId
+StudentUSI
 </v>
       </c>
     </row>
@@ -40582,7 +40595,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I699" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.StudentSchoolAssociationSpecialEnrollment
+        <v xml:space="preserve">arizona.StudentSchoolAssociationSpecialEnrollment
 EntryDate [DATE] NOT NULL
 SchoolId [INT] NOT NULL
 SpecialEnrollmentStartDate [DATE] NOT NULL
@@ -40666,7 +40679,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I700" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.StudentSchoolAssociationTuitionPayer
+        <v xml:space="preserve">arizona.StudentSchoolAssociationTuitionPayer
 EntryDate [DATE] NOT NULL
 PayerStartDate [DATE] NOT NULL
 SchoolId [INT] NOT NULL
@@ -40775,7 +40788,7 @@
 &lt;/xs:complexType&gt;</v>
       </c>
       <c r="I701" t="str" xml:space="preserve">
-        <v xml:space="preserve">az.Track
+        <v xml:space="preserve">arizona.Track
 TrackLocalEducationAgencyId [INT] NOT NULL
 TrackNumberDescriptorId [INT] NOT NULL
 TrackSchoolId [INT] NOT NULL

</xml_diff>